<commit_message>
Add new form for producers
</commit_message>
<xml_diff>
--- a/xlsforms/producer.xlsx
+++ b/xlsforms/producer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="84">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -39,6 +39,9 @@
     <t xml:space="preserve">constraint</t>
   </si>
   <si>
+    <t xml:space="preserve">hint</t>
+  </si>
+  <si>
     <t xml:space="preserve">string</t>
   </si>
   <si>
@@ -90,7 +93,148 @@
     <t xml:space="preserve">GPS Accuracy</t>
   </si>
   <si>
+    <t xml:space="preserve">note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please give some information about your products if they are in the list below.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">begin repeat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delivery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wq:initial(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product  delivered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wq:ForeignKey("ingredient.Ingredient")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shop delivered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wq:ForeignKey("shop.Shop")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity (kg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you deliver this product regularly, please insert the delivery frequency, e.g. once per week.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price per item/kg (PLN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one production_choices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production_mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mode of production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distance_to_shop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distance to shop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To calculate the distance you can use the line tool in the map above.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one yes_no_uncertain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biodegradable_product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was it biodegradable?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recyclable_product_package</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was it in recycling packages?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end repeat</t>
+  </si>
+  <si>
     <t xml:space="preserve">list name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production_choices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">organic_certificate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organic with certificate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">organic_no_certificate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organic without certificate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">traditional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traditional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">industrial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Industrial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes_no_uncertain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uncertain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don‘t know</t>
   </si>
   <si>
     <t xml:space="preserve">location_choices</t>
@@ -262,7 +406,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -293,6 +437,26 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -388,15 +552,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ25"/>
+  <dimension ref="A1:AMJ35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="1" width="31.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="31.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="52.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="36.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="8" style="1" width="31.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
@@ -418,7 +586,9 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="4"/>
       <c r="H1" s="5"/>
       <c r="AMH1" s="1"/>
@@ -427,118 +597,272 @@
     </row>
     <row r="2" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
     </row>
     <row r="4" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G4" s="4"/>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="0"/>
+      <c r="E6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" s="0"/>
-    </row>
-    <row r="10" s="7" customFormat="true" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E9" s="0"/>
+    </row>
+    <row r="10" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G10" s="4"/>
       <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="0"/>
+      <c r="E11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="0"/>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="0"/>
+      <c r="F16" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="0"/>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="0"/>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" customFormat="false" ht="26.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="0"/>
+      <c r="F19" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="0"/>
+    </row>
+    <row r="23" s="7" customFormat="true" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G23" s="4"/>
+      <c r="AMJ23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -564,6 +888,16 @@
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -580,78 +914,149 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1048576"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="31.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="28.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="81.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="8" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="31.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="28.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="13" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="0"/>
+        <v>57</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="0"/>
+        <v>59</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -675,8 +1080,8 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -690,34 +1095,34 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>34</v>
+      <c r="A1" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="11" t="n">
+      <c r="A2" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
Separate producer and producer info
</commit_message>
<xml_diff>
--- a/xlsforms/producer.xlsx
+++ b/xlsforms/producer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -93,148 +93,7 @@
     <t xml:space="preserve">GPS Accuracy</t>
   </si>
   <si>
-    <t xml:space="preserve">note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please give some information about your products if they are in the list below.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">begin repeat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">delivery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wq:initial(1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product  delivered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wq:ForeignKey("ingredient.Ingredient")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shop delivered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wq:ForeignKey("shop.Shop")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantity (kg)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">frequency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frequency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If you deliver this product regularly, please insert the delivery frequency, e.g. once per week.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price per item/kg (PLN)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one production_choices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">production_mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mode of production</t>
-  </si>
-  <si>
-    <t xml:space="preserve">distance_to_shop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distance to shop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To calculate the distance you can use the line tool in the map above.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one yes_no_uncertain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biodegradable_product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Was it biodegradable?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">recyclable_product_package</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Was it in recycling packages?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end repeat</t>
-  </si>
-  <si>
     <t xml:space="preserve">list name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">production_choices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">organic_certificate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organic with certificate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">organic_no_certificate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organic without certificate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">traditional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Traditional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">industrial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Industrial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes_no_uncertain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uncertain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Don‘t know</t>
   </si>
   <si>
     <t xml:space="preserve">location_choices</t>
@@ -406,7 +265,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -437,26 +296,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -552,10 +391,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ35"/>
+  <dimension ref="A1:AMJ34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -694,175 +533,30 @@
       <c r="G10" s="4"/>
       <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="0"/>
-      <c r="E11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="0"/>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="0"/>
-      <c r="F16" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="0"/>
-      <c r="F17" s="10"/>
-    </row>
-    <row r="18" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="0"/>
-      <c r="F18" s="10"/>
-    </row>
-    <row r="19" customFormat="false" ht="26.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="0"/>
-      <c r="F19" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="0"/>
-    </row>
-    <row r="23" s="7" customFormat="true" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G23" s="4"/>
-      <c r="AMJ23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="26.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -897,7 +591,6 @@
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -916,143 +609,73 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="31.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="28.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="20.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="13" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="31.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="28.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="8" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1080,7 +703,7 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1095,34 +718,34 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>82</v>
+      <c r="A1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="16" t="n">
+      <c r="A2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="16"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
Change producer (add fields + add initial producer list)
</commit_message>
<xml_diff>
--- a/xlsforms/producer.xlsx
+++ b/xlsforms/producer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -48,10 +48,37 @@
     <t xml:space="preserve">Name </t>
   </si>
   <si>
-    <t xml:space="preserve">adress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adress</t>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main product(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website</t>
   </si>
   <si>
     <t xml:space="preserve">select_one location_choices</t>
@@ -265,7 +292,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -295,6 +322,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -391,10 +426,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ34"/>
+  <dimension ref="A1:AMJ40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -452,116 +487,179 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D3" s="0"/>
       <c r="E3" s="0"/>
     </row>
-    <row r="4" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G4" s="4"/>
-      <c r="AMJ4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+    <row r="4" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
+    </row>
+    <row r="5" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G5" s="4"/>
+      <c r="AMJ5" s="0"/>
+    </row>
+    <row r="6" s="8" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="0"/>
-      <c r="E5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="G6" s="9"/>
+      <c r="AMJ6" s="9"/>
+    </row>
+    <row r="7" s="8" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="G7" s="9"/>
+      <c r="AMJ7" s="9"/>
+    </row>
+    <row r="8" s="8" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="0"/>
-      <c r="E6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="G8" s="9"/>
+      <c r="AMJ8" s="9"/>
+    </row>
+    <row r="9" s="8" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="0"/>
-      <c r="E7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="0"/>
-      <c r="E9" s="0"/>
+      <c r="G9" s="9"/>
+      <c r="AMJ9" s="9"/>
     </row>
     <row r="10" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G10" s="4"/>
       <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="26.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="0"/>
+      <c r="E11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="0"/>
+      <c r="E15" s="0"/>
+    </row>
+    <row r="16" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G16" s="4"/>
+      <c r="AMJ16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="26.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -591,6 +689,12 @@
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -609,61 +713,61 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A6:C9 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="31.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="28.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="20.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="8" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="31.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="28.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="10" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -704,7 +808,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="A6:C9 A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -718,34 +822,34 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>35</v>
+      <c r="A1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="11" t="n">
+      <c r="A2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
Add question about kindergarten to shop/producer
</commit_message>
<xml_diff>
--- a/xlsforms/producer.xlsx
+++ b/xlsforms/producer.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -57,6 +57,15 @@
     <t xml:space="preserve">Main product(s)</t>
   </si>
   <si>
+    <t xml:space="preserve">select_one yes_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kindergarten_supplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do kindergartens use products from here?</t>
+  </si>
+  <si>
     <t xml:space="preserve">address</t>
   </si>
   <si>
@@ -142,6 +151,21 @@
   </si>
   <si>
     <t xml:space="preserve">Enter Manually</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
   </si>
   <si>
     <t xml:space="preserve">form_title</t>
@@ -292,7 +316,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -322,14 +346,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -426,10 +442,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ40"/>
+  <dimension ref="A1:AMJ41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6:C9"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -508,78 +524,70 @@
       <c r="D4" s="0"/>
       <c r="E4" s="0"/>
     </row>
-    <row r="5" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G5" s="4"/>
-      <c r="AMJ5" s="0"/>
-    </row>
-    <row r="6" s="8" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="5" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="AMJ6" s="9"/>
-    </row>
-    <row r="7" s="8" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+    </row>
+    <row r="6" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G6" s="4"/>
+      <c r="AMJ6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="AMJ7" s="9"/>
-    </row>
-    <row r="8" s="8" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="AMJ8" s="9"/>
-    </row>
-    <row r="9" s="8" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="AMJ9" s="9"/>
-    </row>
-    <row r="10" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G10" s="4"/>
-      <c r="AMJ10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="0"/>
-      <c r="E11" s="0"/>
+    </row>
+    <row r="11" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G11" s="4"/>
+      <c r="AMJ11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -609,58 +617,70 @@
     </row>
     <row r="14" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14" s="0"/>
       <c r="E14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15" s="0"/>
       <c r="E15" s="0"/>
     </row>
-    <row r="16" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G16" s="4"/>
-      <c r="AMJ16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="0"/>
+      <c r="E16" s="0"/>
+    </row>
+    <row r="17" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G17" s="4"/>
+      <c r="AMJ17" s="0"/>
+    </row>
     <row r="18" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="26.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="26.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -695,6 +715,7 @@
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -714,64 +735,84 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A6:C9 A2"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="31.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="28.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="20.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="10" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="31.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="28.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="8" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -808,7 +849,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="A6:C9 A10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -822,34 +863,34 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>44</v>
+      <c r="A1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="13" t="n">
+      <c r="A2" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="13"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
Change field name 'type' to 'short description' in producer
</commit_message>
<xml_diff>
--- a/xlsforms/producer.xlsx
+++ b/xlsforms/producer.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -48,7 +48,10 @@
     <t xml:space="preserve">Name </t>
   </si>
   <si>
-    <t xml:space="preserve">Type</t>
+    <t xml:space="preserve">short_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Short description</t>
   </si>
   <si>
     <t xml:space="preserve">product</t>
@@ -445,7 +448,7 @@
   <dimension ref="A1:AMJ41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -503,10 +506,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="0"/>
       <c r="E3" s="0"/>
@@ -516,23 +519,23 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="0"/>
       <c r="E4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0"/>
       <c r="E5" s="0"/>
@@ -546,10 +549,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -557,10 +560,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -568,10 +571,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -579,10 +582,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -591,65 +594,65 @@
     </row>
     <row r="12" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D13" s="0"/>
       <c r="E13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D14" s="0"/>
       <c r="E14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D15" s="0"/>
       <c r="E15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D16" s="0"/>
       <c r="E16" s="0"/>
@@ -749,7 +752,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>1</v>
@@ -760,57 +763,57 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -864,28 +867,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D2" s="11" t="n">
         <v>1</v>

</xml_diff>